<commit_message>
20240411 jjw -운영소스 머지
</commit_message>
<xml_diff>
--- a/src/main/resources/static/files/20230808_COW_RECV_DNA.xlsx
+++ b/src/main/resources/static/files/20230808_COW_RECV_DNA.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SynologyDrive\스마트가축시장\엑셀업로드\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SynologyDrive\스마트가축시장\소스이관\20230913\nhlvaca\src\main\resources\static\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A663C0-EEBF-4951-9451-D2E4BD5C3155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE401C80-CE8B-4953-99F1-FB0F8C120081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6150" yWindow="2910" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
   <si>
     <t>경매일자</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -87,20 +87,6 @@
   </si>
   <si>
     <t>일치</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>361443-1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>충남0908</t>
-  </si>
-  <si>
-    <t>경기0831</t>
-  </si>
-  <si>
-    <t>4299-1</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -556,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J3:J4"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -644,22 +630,31 @@
         <v>45120</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="5">
-        <v>410002302815139</v>
+        <v>410002097593472</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="G3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="5">
+        <v>410002302453656</v>
+      </c>
       <c r="I3" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -667,22 +662,31 @@
         <v>45120</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="5">
-        <v>410000186355772</v>
+        <v>410002087167466</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="G4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="5">
+        <v>410002076325065</v>
+      </c>
       <c r="I4" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -690,25 +694,25 @@
         <v>45120</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="5">
-        <v>410002097593472</v>
+        <v>410002104585148</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H5" s="5">
-        <v>410002302453656</v>
+        <v>410002302442839</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>14</v>
@@ -722,25 +726,25 @@
         <v>45120</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="5">
-        <v>410002087167466</v>
+        <v>410002098117304</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H6" s="5">
-        <v>410002076325065</v>
+        <v>410002036985337</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>14</v>
@@ -754,25 +758,25 @@
         <v>45120</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E7" s="5">
-        <v>410002104585148</v>
+        <v>410002067321273</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="H7" s="5">
-        <v>410002302442839</v>
+        <v>410002044173050</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>14</v>
@@ -786,94 +790,30 @@
         <v>45120</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="5">
-        <v>410002098117304</v>
+      <c r="E8" s="8">
+        <v>410002044173050</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H8" s="5">
-        <v>410002036985337</v>
+        <v>410000182485992</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
-        <v>45120</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="5">
-        <v>410002067321273</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H9" s="5">
-        <v>410002044173050</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
-        <v>45120</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="8">
-        <v>410002044173050</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H10" s="5">
-        <v>410000182485992</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" s="1" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>